<commit_message>
Arreglo de nuevas funcionalidades para el cliente
</commit_message>
<xml_diff>
--- a/exports/guias_sesion_20250807.xlsx
+++ b/exports/guias_sesion_20250807.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E105"/>
+  <dimension ref="A1:E109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,17 +473,17 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:19:21</t>
         </is>
       </c>
     </row>
@@ -500,17 +500,17 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
@@ -527,17 +527,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
@@ -554,17 +554,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
@@ -581,17 +581,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
@@ -608,17 +608,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
@@ -635,17 +635,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
@@ -662,17 +662,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
@@ -689,17 +689,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
@@ -716,17 +716,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
@@ -743,17 +743,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
@@ -770,17 +770,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
@@ -797,17 +797,17 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
@@ -824,17 +824,17 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
@@ -851,17 +851,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
@@ -878,17 +878,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
@@ -905,17 +905,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
@@ -932,17 +932,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
@@ -959,17 +959,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
@@ -986,17 +986,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
@@ -1013,17 +1013,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
@@ -1040,17 +1040,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
@@ -1067,17 +1067,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
@@ -1094,17 +1094,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
@@ -1121,17 +1121,17 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
@@ -1148,17 +1148,17 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
@@ -1175,17 +1175,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
@@ -1202,17 +1202,17 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
@@ -1229,17 +1229,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
@@ -1256,17 +1256,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
@@ -1283,17 +1283,17 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
@@ -1310,17 +1310,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
@@ -1337,17 +1337,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
@@ -1364,17 +1364,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
@@ -1391,17 +1391,17 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
@@ -1418,17 +1418,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
@@ -1445,17 +1445,17 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
@@ -1472,1799 +1472,1907 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>TBA323067752726</t>
+          <t>TBA323067483217</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>BOG0011142784</t>
+          <t>BOG0011142791</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>TBA323067483217</t>
+          <t>TBA323067481425</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>BOG0011142791</t>
+          <t>BOG0011142731</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>TBA323067481425</t>
+          <t>TBA323067379935</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>BOG0011142731</t>
+          <t>BOG0011142733</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>TBA323067379935</t>
+          <t>TBA323067215546</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>BOG0011142733</t>
+          <t>BOG0011142724</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>TBA323067215546</t>
+          <t>TBA323066955577</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>BOG0011142724</t>
+          <t>BOG0011142932</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>TBA323066955577</t>
+          <t>TBA323065748432</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>BOG0011142932</t>
+          <t>BOG0011142943</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>TBA323065748432</t>
+          <t>TBA323065514270</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>BOG0011142943</t>
+          <t>BOG0011142769</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>TBA323065514270</t>
+          <t>TBA323065354447</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>BOG0011142769</t>
+          <t>BOG0011142788</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>TBA323065354447</t>
+          <t>TBA323065189260</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>BOG0011142788</t>
+          <t>BOG0011142716</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>TBA323065189260</t>
+          <t>TBA323064949443</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>BOG0011142716</t>
+          <t>BOG0011142740</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>TBA323064949443</t>
+          <t>TBA323064833422</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>BOG0011142740</t>
+          <t>BOG0011142721</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>TBA323064833422</t>
+          <t>TBA323064773485</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>BOG0011142721</t>
+          <t>BOG0011142785</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>TBA323064773485</t>
+          <t>TBA323064442166</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>BOG0011142785</t>
+          <t>BOG0011142794</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>TBA323064442166</t>
+          <t>TBA323060264752</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>BOG0011142794</t>
+          <t>BOG0011142778</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>TBA323060264752</t>
+          <t>TBA323060200298</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>BOG0011142778</t>
+          <t>BOG0011142782</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>TBA323060200298</t>
+          <t>TBA323060175410</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>BOG0011142782</t>
+          <t>BOG0011142803</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>TBA323060175410</t>
+          <t>TBA323060080360</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>BOG0011142803</t>
+          <t>BOG0011142936</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>TBA323060080360</t>
+          <t>TBA323059932389</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>BOG0011142936</t>
+          <t>BOG0011142735</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>TBA323059932389</t>
+          <t>TBA323056168803</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>BOG0011142735</t>
+          <t>BOG0011142790</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>TBA323056168803</t>
+          <t>TBA323054173890</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>BOG0011142790</t>
+          <t>BOG0011142797</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>TBA323054173890</t>
+          <t>TBA323054042345</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>BOG0011142797</t>
+          <t>BOG0011142792</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>TBA323054042345</t>
+          <t>TBA323051817440</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>BOG0011142792</t>
+          <t>BOG0011142779</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>TBA323051817440</t>
+          <t>TBA323050760089</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>BOG0011142779</t>
+          <t>BOG0011142804</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>TBA323050760089</t>
+          <t>TBA323050436599</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>BOG0011142804</t>
+          <t>BOG0011142548</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>TBA323050436599</t>
+          <t>TBA323050306127</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>BOG0011142548</t>
+          <t>BOG0011142635</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>TBA323050306127</t>
+          <t>TBA323049275611</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>BOG0011142635</t>
+          <t>BOG0011142801</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>TBA323049275611</t>
+          <t>TBA323048756559</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>BOG0011142801</t>
+          <t>BOG0011142789</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>TBA323048756559</t>
+          <t>TBA323047725294</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>BOG0011142789</t>
+          <t>BOG0011142627</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>TBA323047725294</t>
+          <t>TBA323046640835</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>BOG0011142627</t>
+          <t>BOG0011142781</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>TBA323047693856</t>
+          <t>TBA323046489893</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>BOG0011142737</t>
+          <t>BOG0011142639</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>TBA323046640835</t>
+          <t>TBA323045835654</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>BOG0011142781</t>
+          <t>BOG0011142614</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>TBA323046489893</t>
+          <t>TBA323045525229</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>BOG0011142639</t>
+          <t>BOG0011142592</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>TBA323046215869</t>
+          <t>TBA323045331849</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>BOG0011142646</t>
+          <t>BOG0011142640</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>TBA323045835654</t>
+          <t>TBA323044998566</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>BOG0011142614</t>
+          <t>BOG0011142642</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>TBA323045525229</t>
+          <t>TBA323044603885</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>BOG0011142592</t>
+          <t>BOG0011142616</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>TBA323045331849</t>
+          <t>TBA323044225455</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>BOG0011142640</t>
+          <t>BOG0011142624</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>TBA323044998566</t>
+          <t>TBA323043605568</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>BOG0011142642</t>
+          <t>BOG0011142605</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>TBA323044603885</t>
+          <t>TBA323043396001</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>BOG0011142616</t>
+          <t>BOG0011142641</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>TBA323044225455</t>
+          <t>TBA323042863218</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>BOG0011142624</t>
+          <t>BOG0011142608</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>TBA323043605568</t>
+          <t>TBA323042358097</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>BOG0011142605</t>
+          <t>BOG0011142771</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>TBA323043552239</t>
+          <t>TBA323041079098</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>BOG0011142691</t>
+          <t>BOG0011142591</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>TBA323043396001</t>
+          <t>TBA323040906555</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>BOG0011142641</t>
+          <t>BOG0011142622</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>TBA323042863218</t>
+          <t>TBA323040840858</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>BOG0011142608</t>
+          <t>BOG0011142770</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>TBA323042358097</t>
+          <t>TBA323040511974</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>BOG0011142771</t>
+          <t>BOG0011142765</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>TBA323041521274</t>
+          <t>TBA323040436706</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>BOG0011142780</t>
+          <t>BOG0011142643</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>TBA323041079098</t>
+          <t>TBA323040228272</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>BOG0011142591</t>
+          <t>BOG0011142621</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>TBA323040906555</t>
+          <t>TBA323039927821</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>BOG0011142622</t>
+          <t>BOG0011142663</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>TBA323040840858</t>
+          <t>TBA323039720003</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>BOG0011142770</t>
+          <t>BOG0011142571</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>TBA323040511974</t>
+          <t>TBA323039687648</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>BOG0011142765</t>
+          <t>BOG0011142623</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>TBA323040436706</t>
+          <t>TBA323039654387</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>BOG0011142643</t>
+          <t>BOG0011142777</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>TBA323040228272</t>
+          <t>TBA323039441832</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>BOG0011142621</t>
+          <t>BOG0011142787</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>TBA323039982955</t>
+          <t>TBA323039298468</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>BOG0011142607</t>
+          <t>BOG0011142617</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>TBA323039927821</t>
+          <t>TBA323039084420</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>BOG0011142663</t>
+          <t>BOG0011142625</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>TBA323039720003</t>
+          <t>TBA323039003113</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>BOG0011142571</t>
+          <t>BOG0011142647</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>TBA323039687648</t>
+          <t>TBA323038796730</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>BOG0011142623</t>
+          <t>BOG0011142633</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>TBA323039654387</t>
+          <t>TBA323038688439</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>BOG0011142777</t>
+          <t>BOG0011142648</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>TBA323039441832</t>
+          <t>TBA323038429030</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>BOG0011142787</t>
+          <t>BOG0011142618</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>TBA323039355408</t>
+          <t>TBA323037911002</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>BOG0011142774</t>
+          <t>BOG0011142645</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESCANEADO</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:10:26</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>TBA323039298468</t>
+          <t>TBA323067752726</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>BOG0011142617</t>
+          <t>BOG0011142784</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>RECIBIDO</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:08:12</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>TBA323039084420</t>
+          <t>TBA323046215869</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>BOG0011142625</t>
+          <t>BOG0011142646</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>RECIBIDO</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:05:04</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>TBA323039003113</t>
+          <t>TBA323047693856</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>BOG0011142647</t>
+          <t>BOG0011142737</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>RECIBIDO</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:04:54</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>TBA323038796730</t>
+          <t>789</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>BOG0011142633</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:04:25</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESPERADO</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:04:25</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>TBA323038688439</t>
+          <t>4657</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>BOG0011142648</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:02:42</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESPERADO</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:02:42</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>TBA323038545754</t>
+          <t>14567</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>BOG0011142620</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:00:19</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESPERADO</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 04:00:19</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>TBA323038429030</t>
+          <t>1234</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>BOG0011142618</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:59:54</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>NO ESPERADO</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:59:54</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>TBA323037911002</t>
+          <t>TBA323043552239</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>BOG0011142645</t>
+          <t>BOG0011142691</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:57:05</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>NO RECIBIDO</t>
+          <t>RECIBIDO</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>2025-08-08 00:50:06</t>
+          <t>2025-08-08 03:59:46</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>TBA323041521274</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>BOG0011142780</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>2025-08-08 03:57:05</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>RECIBIDO</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>2025-08-08 03:59:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>TBA323039982955</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>BOG0011142607</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>2025-08-08 03:57:05</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>RECIBIDO</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>2025-08-08 03:59:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>TBA323039355408</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>BOG0011142774</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>2025-08-08 03:57:05</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>RECIBIDO</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>2025-08-08 03:59:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>TBA323038545754</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>BOG0011142620</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>2025-08-08 03:57:05</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>RECIBIDO</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>2025-08-08 03:58:53</t>
         </is>
       </c>
     </row>

</xml_diff>